<commit_message>
MISTI, MISTII, Pavlov2020, XSVT, Reversflow LCS, Speckle matching
</commit_message>
<xml_diff>
--- a/Experiment.xlsx
+++ b/Experiment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clement.capdeville\Documents\GitHub\MoBI_plugin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259DC480-8D08-40B1-98D9-BDE34AB7ECC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFDB0DBF-D097-4424-9643-29191E3CF2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="8520" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="40">
   <si>
     <t>Paramètres</t>
   </si>
@@ -96,15 +96,9 @@
     <t>MISTI</t>
   </si>
   <si>
-    <t>Pavlov2080</t>
-  </si>
-  <si>
     <t>XSVT</t>
   </si>
   <si>
-    <t>ReversflowVCS</t>
-  </si>
-  <si>
     <t>Speckle Matching</t>
   </si>
   <si>
@@ -145,6 +139,21 @@
   </si>
   <si>
     <t>source_size</t>
+  </si>
+  <si>
+    <t>Pavlov2020</t>
+  </si>
+  <si>
+    <t>XSVT_median_filter</t>
+  </si>
+  <si>
+    <t>XSVT_Nw</t>
+  </si>
+  <si>
+    <t>ReversflowLCS</t>
+  </si>
+  <si>
+    <t>umpaNw</t>
   </si>
 </sst>
 </file>
@@ -197,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -206,10 +215,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -261,20 +267,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3937535-0727-4AA2-90D2-3C52474DAEB5}" name="Tableau1" displayName="Tableau1" ref="A1:K21" totalsRowShown="0">
-  <autoFilter ref="A1:K21" xr:uid="{E3937535-0727-4AA2-90D2-3C52474DAEB5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E3937535-0727-4AA2-90D2-3C52474DAEB5}" name="Tableau1" displayName="Tableau1" ref="A1:K24" totalsRowShown="0">
+  <autoFilter ref="A1:K24" xr:uid="{E3937535-0727-4AA2-90D2-3C52474DAEB5}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{41D8092C-CECE-4506-9B1D-29E20835EAD2}" name="Paramètres"/>
     <tableColumn id="2" xr3:uid="{9D6EBFCF-A114-4DC8-BFFD-799413A2F680}" name="LCS" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{16F1FBC5-BBB7-4E37-9805-39BB79ADD75E}" name="LCS DF" dataDxfId="8"/>
     <tableColumn id="4" xr3:uid="{D7620047-C8EC-472D-B7CD-3969A182437A}" name="LCS DIR DF" dataDxfId="7"/>
     <tableColumn id="5" xr3:uid="{3BCAB51E-CD9A-4C99-86E9-FD4AD118D5F6}" name="MISTI" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{1F5F5DD4-6592-4570-9099-7E3957477BAE}" name="MISTII 1" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{0B26955D-FF86-4443-A418-C6DD0F231634}" name="MISTII 2" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{E2B9F18C-EC10-4A6C-8F63-F9BC6B2AB9A2}" name="Pavlov2080" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{42093672-9E92-4024-B543-7E54D51BDE55}" name="XSVT" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{FCF908AE-7A5E-4FC5-8FD3-30BD882F8348}" name="ReversflowVCS" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{050E3C2A-F666-48AB-B51E-7DCA5E394F10}" name="Speckle Matching" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{1F5F5DD4-6592-4570-9099-7E3957477BAE}" name="MISTII 1" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{0B26955D-FF86-4443-A418-C6DD0F231634}" name="MISTII 2" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{E2B9F18C-EC10-4A6C-8F63-F9BC6B2AB9A2}" name="Pavlov2020" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{42093672-9E92-4024-B543-7E54D51BDE55}" name="XSVT" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{FCF908AE-7A5E-4FC5-8FD3-30BD882F8348}" name="ReversflowLCS" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{050E3C2A-F666-48AB-B51E-7DCA5E394F10}" name="Speckle Matching" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -543,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -580,210 +586,210 @@
         <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
         <v>21</v>
-      </c>
-      <c r="J1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>29</v>
+      <c r="B2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>30</v>
+      <c r="B3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>30</v>
+      <c r="B4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>30</v>
+      <c r="B5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>30</v>
+      <c r="B6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="B7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -794,13 +800,13 @@
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="B8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -811,134 +817,158 @@
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>32</v>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="J9" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>31</v>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>31</v>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
@@ -947,22 +977,22 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
+      </c>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -970,22 +1000,22 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -993,22 +1023,22 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1016,19 +1046,19 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -1037,22 +1067,22 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1060,7 +1090,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1069,34 +1099,97 @@
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
+      <c r="F24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>